<commit_message>
Working on loading day probabilities from excel
</commit_message>
<xml_diff>
--- a/src/main/resources/Daten.xlsx
+++ b/src/main/resources/Daten.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\findu\CloudStation\Dokumente\Uni\Masterthesis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CloudStation\java-development\MasterThesis\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="38" windowWidth="15960" windowHeight="8858" firstSheet="3" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="45" windowWidth="15960" windowHeight="8865" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Otitis externa" sheetId="1" r:id="rId1"/>
@@ -511,7 +511,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="84">
   <si>
     <t>Krankheit:</t>
   </si>
@@ -670,9 +670,6 @@
   </si>
   <si>
     <t>(Werte in % bzw. *Multiplikator)</t>
-  </si>
-  <si>
-    <t>Cer. Obt.</t>
   </si>
   <si>
     <t>Zoster oticus</t>
@@ -2271,15 +2268,15 @@
       <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="12.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="12.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.46484375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.86328125" style="1" customWidth="1"/>
-    <col min="3" max="21" width="9.19921875" style="1" customWidth="1"/>
-    <col min="22" max="256" width="8.86328125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="43.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" style="1" customWidth="1"/>
+    <col min="3" max="21" width="9.140625" style="1" customWidth="1"/>
+    <col min="22" max="256" width="8.85546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="17" customHeight="1">
+    <row r="1" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2310,7 +2307,7 @@
       <c r="T1" s="7"/>
       <c r="U1" s="7"/>
     </row>
-    <row r="2" spans="1:21" ht="17" customHeight="1">
+    <row r="2" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A2" s="8"/>
       <c r="B2" s="9"/>
       <c r="C2" s="9"/>
@@ -2454,7 +2451,7 @@
       <c r="T4" s="38"/>
       <c r="U4" s="38"/>
     </row>
-    <row r="5" spans="1:21" ht="17" customHeight="1">
+    <row r="5" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A5" s="18"/>
       <c r="B5" s="19"/>
       <c r="C5" s="20"/>
@@ -2477,7 +2474,7 @@
       <c r="T5" s="38"/>
       <c r="U5" s="38"/>
     </row>
-    <row r="6" spans="1:21" ht="17" customHeight="1">
+    <row r="6" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A6" s="14" t="s">
         <v>20</v>
       </c>
@@ -2543,7 +2540,7 @@
       <c r="T6" s="38"/>
       <c r="U6" s="38"/>
     </row>
-    <row r="7" spans="1:21" ht="17" customHeight="1">
+    <row r="7" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A7" s="14" t="s">
         <v>21</v>
       </c>
@@ -2609,7 +2606,7 @@
       <c r="T7" s="38"/>
       <c r="U7" s="38"/>
     </row>
-    <row r="8" spans="1:21" ht="17" customHeight="1">
+    <row r="8" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A8" s="14" t="s">
         <v>22</v>
       </c>
@@ -2675,7 +2672,7 @@
       <c r="T8" s="38"/>
       <c r="U8" s="38"/>
     </row>
-    <row r="9" spans="1:21" ht="17" customHeight="1">
+    <row r="9" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A9" s="14" t="s">
         <v>23</v>
       </c>
@@ -2741,7 +2738,7 @@
       <c r="T9" s="38"/>
       <c r="U9" s="38"/>
     </row>
-    <row r="10" spans="1:21" ht="17" customHeight="1">
+    <row r="10" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A10" s="14" t="s">
         <v>24</v>
       </c>
@@ -2807,7 +2804,7 @@
       <c r="T10" s="38"/>
       <c r="U10" s="38"/>
     </row>
-    <row r="11" spans="1:21" ht="17" customHeight="1">
+    <row r="11" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A11" s="14" t="s">
         <v>25</v>
       </c>
@@ -2873,7 +2870,7 @@
       <c r="T11" s="38"/>
       <c r="U11" s="38"/>
     </row>
-    <row r="12" spans="1:21" ht="17" customHeight="1">
+    <row r="12" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A12" s="14" t="s">
         <v>26</v>
       </c>
@@ -2939,7 +2936,7 @@
       <c r="T12" s="38"/>
       <c r="U12" s="38"/>
     </row>
-    <row r="13" spans="1:21" ht="17" customHeight="1">
+    <row r="13" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A13" s="14" t="s">
         <v>27</v>
       </c>
@@ -3005,7 +3002,7 @@
       <c r="T13" s="38"/>
       <c r="U13" s="38"/>
     </row>
-    <row r="14" spans="1:21" ht="17" customHeight="1">
+    <row r="14" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A14" s="14" t="s">
         <v>28</v>
       </c>
@@ -3071,7 +3068,7 @@
       <c r="T14" s="38"/>
       <c r="U14" s="38"/>
     </row>
-    <row r="15" spans="1:21" ht="17" customHeight="1">
+    <row r="15" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A15" s="14" t="s">
         <v>29</v>
       </c>
@@ -3137,7 +3134,7 @@
       <c r="T15" s="38"/>
       <c r="U15" s="38"/>
     </row>
-    <row r="16" spans="1:21" ht="17" customHeight="1">
+    <row r="16" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A16" s="14" t="s">
         <v>30</v>
       </c>
@@ -3335,7 +3332,7 @@
       <c r="T18" s="22"/>
       <c r="U18" s="22"/>
     </row>
-    <row r="19" spans="1:21" ht="17" customHeight="1">
+    <row r="19" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A19" s="14" t="s">
         <v>33</v>
       </c>
@@ -3401,7 +3398,7 @@
       <c r="T19" s="7"/>
       <c r="U19" s="7"/>
     </row>
-    <row r="20" spans="1:21" ht="17" customHeight="1">
+    <row r="20" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A20" s="14" t="s">
         <v>34</v>
       </c>
@@ -3467,7 +3464,7 @@
       <c r="T20" s="7"/>
       <c r="U20" s="7"/>
     </row>
-    <row r="21" spans="1:21" ht="17" customHeight="1">
+    <row r="21" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A21" s="14" t="s">
         <v>35</v>
       </c>
@@ -3533,7 +3530,7 @@
       <c r="T21" s="7"/>
       <c r="U21" s="7"/>
     </row>
-    <row r="22" spans="1:21" ht="17" customHeight="1">
+    <row r="22" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A22" s="14" t="s">
         <v>36</v>
       </c>
@@ -3599,7 +3596,7 @@
       <c r="T22" s="7"/>
       <c r="U22" s="7"/>
     </row>
-    <row r="23" spans="1:21" ht="17" customHeight="1">
+    <row r="23" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A23" s="14" t="s">
         <v>37</v>
       </c>
@@ -3665,7 +3662,7 @@
       <c r="T23" s="7"/>
       <c r="U23" s="7"/>
     </row>
-    <row r="24" spans="1:21" ht="17" customHeight="1">
+    <row r="24" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A24" s="14" t="s">
         <v>38</v>
       </c>
@@ -3731,7 +3728,7 @@
       <c r="T24" s="7"/>
       <c r="U24" s="7"/>
     </row>
-    <row r="25" spans="1:21" ht="17" customHeight="1">
+    <row r="25" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A25" s="14" t="s">
         <v>39</v>
       </c>
@@ -3797,7 +3794,7 @@
       <c r="T25" s="7"/>
       <c r="U25" s="7"/>
     </row>
-    <row r="26" spans="1:21" ht="17" customHeight="1">
+    <row r="26" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A26" s="14" t="s">
         <v>40</v>
       </c>
@@ -3863,7 +3860,7 @@
       <c r="T26" s="7"/>
       <c r="U26" s="7"/>
     </row>
-    <row r="27" spans="1:21" ht="17" customHeight="1">
+    <row r="27" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A27" s="14" t="s">
         <v>41</v>
       </c>
@@ -3929,7 +3926,7 @@
       <c r="T27" s="7"/>
       <c r="U27" s="7"/>
     </row>
-    <row r="28" spans="1:21" ht="17" customHeight="1">
+    <row r="28" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A28" s="23"/>
       <c r="B28" s="24"/>
       <c r="C28" s="25">
@@ -4010,26 +4007,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:IV14"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.796875" defaultRowHeight="12.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.85546875" defaultRowHeight="12.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="25" style="34" customWidth="1"/>
-    <col min="2" max="2" width="14.86328125" style="34" customWidth="1"/>
-    <col min="3" max="3" width="9.33203125" style="34" customWidth="1"/>
-    <col min="4" max="4" width="8.86328125" style="34" customWidth="1"/>
-    <col min="5" max="5" width="11.46484375" style="34" customWidth="1"/>
-    <col min="6" max="6" width="10.33203125" style="34" customWidth="1"/>
-    <col min="7" max="7" width="9.6640625" style="34" customWidth="1"/>
-    <col min="8" max="8" width="12.86328125" style="34" customWidth="1"/>
-    <col min="9" max="9" width="14.6640625" style="34" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" style="34" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" style="34" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" style="34" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" style="34" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" style="34" customWidth="1"/>
+    <col min="7" max="7" width="18.140625" style="34" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.85546875" style="34" customWidth="1"/>
+    <col min="9" max="9" width="14.7109375" style="34" customWidth="1"/>
     <col min="10" max="10" width="8" style="34" customWidth="1"/>
-    <col min="11" max="11" width="6.86328125" style="34" customWidth="1"/>
+    <col min="11" max="11" width="6.85546875" style="34" customWidth="1"/>
     <col min="12" max="12" width="8" style="34" customWidth="1"/>
-    <col min="13" max="256" width="11.86328125" style="34" customWidth="1"/>
+    <col min="13" max="256" width="11.85546875" style="34" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="17" customHeight="1">
+    <row r="1" spans="1:12" ht="17.100000000000001" customHeight="1">
       <c r="A1" s="11" t="s">
         <v>52</v>
       </c>
@@ -4049,10 +4048,10 @@
         <v>47</v>
       </c>
       <c r="G1" s="35" t="s">
+        <v>48</v>
+      </c>
+      <c r="H1" s="35" t="s">
         <v>53</v>
-      </c>
-      <c r="H1" s="35" t="s">
-        <v>54</v>
       </c>
       <c r="I1" s="35" t="s">
         <v>50</v>
@@ -4061,15 +4060,15 @@
         <v>51</v>
       </c>
       <c r="K1" s="35" t="s">
+        <v>54</v>
+      </c>
+      <c r="L1" s="35" t="s">
         <v>55</v>
-      </c>
-      <c r="L1" s="35" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="13.7" customHeight="1">
       <c r="A2" s="11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B2" s="8">
         <v>0.1</v>
@@ -4107,7 +4106,7 @@
     </row>
     <row r="3" spans="1:12" ht="13.7" customHeight="1">
       <c r="A3" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B3" s="8">
         <v>1.3</v>
@@ -4145,7 +4144,7 @@
     </row>
     <row r="4" spans="1:12" ht="13.7" customHeight="1">
       <c r="A4" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B4" s="8">
         <v>1</v>
@@ -4183,7 +4182,7 @@
     </row>
     <row r="5" spans="1:12" ht="13.7" customHeight="1">
       <c r="A5" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B5" s="8">
         <v>1.3</v>
@@ -4221,7 +4220,7 @@
     </row>
     <row r="6" spans="1:12" ht="13.7" customHeight="1">
       <c r="A6" s="11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B6" s="8">
         <v>0.7</v>
@@ -4259,306 +4258,306 @@
     </row>
     <row r="7" spans="1:12" ht="13.7" customHeight="1">
       <c r="A7" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="B7" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="C7" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="D7" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="H7" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="D7" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="E7" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="F7" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="G7" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="H7" s="11" t="s">
-        <v>65</v>
-      </c>
       <c r="I7" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J7" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K7" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L7" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="13.7" customHeight="1">
       <c r="A8" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="H8" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="I8" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="J8" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="K8" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="D8" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="E8" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="F8" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="G8" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="H8" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="I8" s="11" t="s">
+      <c r="L8" s="11" t="s">
         <v>67</v>
-      </c>
-      <c r="J8" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="K8" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="L8" s="11" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="13.7" customHeight="1">
       <c r="A9" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="C9" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="B9" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="C9" s="11" t="s">
+      <c r="D9" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="F9" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="D9" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="E9" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="F9" s="11" t="s">
+      <c r="G9" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="G9" s="11" t="s">
-        <v>72</v>
-      </c>
       <c r="H9" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I9" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J9" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K9" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L9" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="13.7" customHeight="1">
       <c r="A10" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="D10" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="E10" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="C10" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="D10" s="11" t="s">
+      <c r="F10" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="H10" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="I10" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="J10" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="E10" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="F10" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="G10" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="H10" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="I10" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="J10" s="11" t="s">
-        <v>75</v>
-      </c>
       <c r="K10" s="11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="L10" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="13.7" customHeight="1">
       <c r="A11" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="C11" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="B11" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="C11" s="11" t="s">
+      <c r="D11" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="F11" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="D11" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="E11" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="F11" s="11" t="s">
-        <v>78</v>
-      </c>
       <c r="G11" s="11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H11" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I11" s="11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J11" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K11" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L11" s="11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="13.7" customHeight="1">
       <c r="A12" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="C12" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="D12" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="E12" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="F12" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="D12" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="E12" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="F12" s="11" t="s">
-        <v>81</v>
-      </c>
       <c r="G12" s="11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H12" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I12" s="11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J12" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K12" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L12" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="13.7" customHeight="1">
       <c r="A13" s="11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B13" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="D13" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="C13" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="D13" s="11" t="s">
-        <v>64</v>
-      </c>
       <c r="E13" s="11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F13" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G13" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H13" s="11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I13" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J13" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K13" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L13" s="11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="13.7" customHeight="1">
       <c r="A14" s="11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D14" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="E14" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="E14" s="11" t="s">
-        <v>64</v>
-      </c>
       <c r="F14" s="11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G14" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H14" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I14" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J14" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K14" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L14" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -4577,20 +4576,20 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.796875" defaultRowHeight="12.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.85546875" defaultRowHeight="12.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="44" style="36" customWidth="1"/>
-    <col min="2" max="2" width="16.33203125" style="36" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" style="36" customWidth="1"/>
     <col min="3" max="3" width="14" style="36" customWidth="1"/>
-    <col min="4" max="6" width="12.33203125" style="36" customWidth="1"/>
-    <col min="7" max="7" width="19.6640625" style="36" customWidth="1"/>
+    <col min="4" max="6" width="12.28515625" style="36" customWidth="1"/>
+    <col min="7" max="7" width="19.7109375" style="36" customWidth="1"/>
     <col min="8" max="8" width="15" style="36" customWidth="1"/>
-    <col min="9" max="9" width="15.6640625" style="36" customWidth="1"/>
-    <col min="10" max="12" width="12.33203125" style="36" customWidth="1"/>
-    <col min="13" max="256" width="11.86328125" style="36" customWidth="1"/>
+    <col min="9" max="9" width="15.7109375" style="36" customWidth="1"/>
+    <col min="10" max="12" width="12.28515625" style="36" customWidth="1"/>
+    <col min="13" max="256" width="11.85546875" style="36" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="17" customHeight="1">
+    <row r="1" spans="1:12" ht="17.100000000000001" customHeight="1">
       <c r="A1" s="11" t="s">
         <v>3</v>
       </c>
@@ -4613,7 +4612,7 @@
         <v>48</v>
       </c>
       <c r="H1" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I1" s="11" t="s">
         <v>50</v>
@@ -4622,13 +4621,13 @@
         <v>51</v>
       </c>
       <c r="K1" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="L1" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="L1" s="11" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="17" customHeight="1">
+    </row>
+    <row r="2" spans="1:12" ht="17.100000000000001" customHeight="1">
       <c r="A2" s="11" t="s">
         <v>20</v>
       </c>
@@ -4666,7 +4665,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="17" customHeight="1">
+    <row r="3" spans="1:12" ht="17.100000000000001" customHeight="1">
       <c r="A3" s="11" t="s">
         <v>21</v>
       </c>
@@ -4704,7 +4703,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="17" customHeight="1">
+    <row r="4" spans="1:12" ht="17.100000000000001" customHeight="1">
       <c r="A4" s="11" t="s">
         <v>22</v>
       </c>
@@ -4742,7 +4741,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="17" customHeight="1">
+    <row r="5" spans="1:12" ht="17.100000000000001" customHeight="1">
       <c r="A5" s="11" t="s">
         <v>23</v>
       </c>
@@ -4780,7 +4779,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="17" customHeight="1">
+    <row r="6" spans="1:12" ht="17.100000000000001" customHeight="1">
       <c r="A6" s="11" t="s">
         <v>24</v>
       </c>
@@ -4818,7 +4817,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="17" customHeight="1">
+    <row r="7" spans="1:12" ht="17.100000000000001" customHeight="1">
       <c r="A7" s="11" t="s">
         <v>25</v>
       </c>
@@ -4856,7 +4855,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="17" customHeight="1">
+    <row r="8" spans="1:12" ht="17.100000000000001" customHeight="1">
       <c r="A8" s="11" t="s">
         <v>26</v>
       </c>
@@ -4894,7 +4893,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="17" customHeight="1">
+    <row r="9" spans="1:12" ht="17.100000000000001" customHeight="1">
       <c r="A9" s="11" t="s">
         <v>27</v>
       </c>
@@ -4932,7 +4931,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="17" customHeight="1">
+    <row r="10" spans="1:12" ht="17.100000000000001" customHeight="1">
       <c r="A10" s="11" t="s">
         <v>28</v>
       </c>
@@ -4970,7 +4969,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="17" customHeight="1">
+    <row r="11" spans="1:12" ht="17.100000000000001" customHeight="1">
       <c r="A11" s="11" t="s">
         <v>29</v>
       </c>
@@ -5008,7 +5007,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="17" customHeight="1">
+    <row r="12" spans="1:12" ht="17.100000000000001" customHeight="1">
       <c r="A12" s="11" t="s">
         <v>30</v>
       </c>
@@ -5046,7 +5045,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="17" customHeight="1">
+    <row r="13" spans="1:12" ht="17.100000000000001" customHeight="1">
       <c r="A13" s="11" t="s">
         <v>31</v>
       </c>
@@ -5084,7 +5083,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="17" customHeight="1">
+    <row r="14" spans="1:12" ht="17.100000000000001" customHeight="1">
       <c r="A14" s="11" t="s">
         <v>32</v>
       </c>
@@ -5122,7 +5121,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="17" customHeight="1">
+    <row r="15" spans="1:12" ht="17.100000000000001" customHeight="1">
       <c r="A15" s="11" t="s">
         <v>33</v>
       </c>
@@ -5160,7 +5159,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="17" customHeight="1">
+    <row r="16" spans="1:12" ht="17.100000000000001" customHeight="1">
       <c r="A16" s="11" t="s">
         <v>34</v>
       </c>
@@ -5198,7 +5197,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="17" customHeight="1">
+    <row r="17" spans="1:12" ht="17.100000000000001" customHeight="1">
       <c r="A17" s="11" t="s">
         <v>35</v>
       </c>
@@ -5236,7 +5235,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="17" customHeight="1">
+    <row r="18" spans="1:12" ht="17.100000000000001" customHeight="1">
       <c r="A18" s="11" t="s">
         <v>36</v>
       </c>
@@ -5271,10 +5270,10 @@
         <v>10</v>
       </c>
       <c r="L18" s="11" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" ht="17" customHeight="1">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="17.100000000000001" customHeight="1">
       <c r="A19" s="11" t="s">
         <v>37</v>
       </c>
@@ -5312,7 +5311,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="17" customHeight="1">
+    <row r="20" spans="1:12" ht="17.100000000000001" customHeight="1">
       <c r="A20" s="11" t="s">
         <v>38</v>
       </c>
@@ -5350,7 +5349,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="17" customHeight="1">
+    <row r="21" spans="1:12" ht="17.100000000000001" customHeight="1">
       <c r="A21" s="11" t="s">
         <v>39</v>
       </c>
@@ -5388,7 +5387,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="17" customHeight="1">
+    <row r="22" spans="1:12" ht="17.100000000000001" customHeight="1">
       <c r="A22" s="11" t="s">
         <v>40</v>
       </c>
@@ -5426,7 +5425,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="17" customHeight="1">
+    <row r="23" spans="1:12" ht="17.100000000000001" customHeight="1">
       <c r="A23" s="7"/>
       <c r="B23" s="8"/>
       <c r="C23" s="8"/>
@@ -5440,7 +5439,7 @@
       <c r="K23" s="7"/>
       <c r="L23" s="7"/>
     </row>
-    <row r="24" spans="1:12" ht="17" customHeight="1">
+    <row r="24" spans="1:12" ht="17.100000000000001" customHeight="1">
       <c r="A24" s="7"/>
       <c r="B24" s="8"/>
       <c r="C24" s="8"/>
@@ -5454,7 +5453,7 @@
       <c r="K24" s="7"/>
       <c r="L24" s="7"/>
     </row>
-    <row r="25" spans="1:12" ht="17" customHeight="1">
+    <row r="25" spans="1:12" ht="17.100000000000001" customHeight="1">
       <c r="A25" s="7"/>
       <c r="B25" s="8"/>
       <c r="C25" s="8"/>
@@ -5485,15 +5484,15 @@
       <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="12.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="12.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.46484375" style="26" customWidth="1"/>
-    <col min="2" max="2" width="10.86328125" style="26" customWidth="1"/>
-    <col min="3" max="21" width="9.19921875" style="26" customWidth="1"/>
-    <col min="22" max="256" width="8.86328125" style="26" customWidth="1"/>
+    <col min="1" max="1" width="43.42578125" style="26" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" style="26" customWidth="1"/>
+    <col min="3" max="21" width="9.140625" style="26" customWidth="1"/>
+    <col min="22" max="256" width="8.85546875" style="26" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="17" customHeight="1">
+    <row r="1" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -5524,7 +5523,7 @@
       <c r="T1" s="7"/>
       <c r="U1" s="7"/>
     </row>
-    <row r="2" spans="1:21" ht="17" customHeight="1">
+    <row r="2" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A2" s="8"/>
       <c r="B2" s="9"/>
       <c r="C2" s="9"/>
@@ -5658,7 +5657,7 @@
       <c r="T4" s="38"/>
       <c r="U4" s="38"/>
     </row>
-    <row r="5" spans="1:21" ht="17" customHeight="1">
+    <row r="5" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A5" s="18"/>
       <c r="B5" s="19"/>
       <c r="C5" s="20"/>
@@ -5681,7 +5680,7 @@
       <c r="T5" s="38"/>
       <c r="U5" s="38"/>
     </row>
-    <row r="6" spans="1:21" ht="17" customHeight="1">
+    <row r="6" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A6" s="14" t="s">
         <v>20</v>
       </c>
@@ -5734,7 +5733,7 @@
       <c r="T6" s="38"/>
       <c r="U6" s="38"/>
     </row>
-    <row r="7" spans="1:21" ht="17" customHeight="1">
+    <row r="7" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A7" s="14" t="s">
         <v>21</v>
       </c>
@@ -5796,7 +5795,7 @@
       <c r="T7" s="38"/>
       <c r="U7" s="38"/>
     </row>
-    <row r="8" spans="1:21" ht="17" customHeight="1">
+    <row r="8" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A8" s="14" t="s">
         <v>22</v>
       </c>
@@ -5862,7 +5861,7 @@
       <c r="T8" s="38"/>
       <c r="U8" s="38"/>
     </row>
-    <row r="9" spans="1:21" ht="17" customHeight="1">
+    <row r="9" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A9" s="14" t="s">
         <v>23</v>
       </c>
@@ -5920,7 +5919,7 @@
       <c r="T9" s="38"/>
       <c r="U9" s="38"/>
     </row>
-    <row r="10" spans="1:21" ht="17" customHeight="1">
+    <row r="10" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A10" s="14" t="s">
         <v>24</v>
       </c>
@@ -5978,7 +5977,7 @@
       <c r="T10" s="38"/>
       <c r="U10" s="38"/>
     </row>
-    <row r="11" spans="1:21" ht="17" customHeight="1">
+    <row r="11" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A11" s="14" t="s">
         <v>25</v>
       </c>
@@ -6036,7 +6035,7 @@
       <c r="T11" s="38"/>
       <c r="U11" s="38"/>
     </row>
-    <row r="12" spans="1:21" ht="17" customHeight="1">
+    <row r="12" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A12" s="14" t="s">
         <v>26</v>
       </c>
@@ -6094,7 +6093,7 @@
       <c r="T12" s="38"/>
       <c r="U12" s="38"/>
     </row>
-    <row r="13" spans="1:21" ht="17" customHeight="1">
+    <row r="13" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A13" s="14" t="s">
         <v>27</v>
       </c>
@@ -6155,7 +6154,7 @@
       <c r="T13" s="38"/>
       <c r="U13" s="38"/>
     </row>
-    <row r="14" spans="1:21" ht="17" customHeight="1">
+    <row r="14" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A14" s="14" t="s">
         <v>28</v>
       </c>
@@ -6218,7 +6217,7 @@
       <c r="T14" s="38"/>
       <c r="U14" s="38"/>
     </row>
-    <row r="15" spans="1:21" ht="17" customHeight="1">
+    <row r="15" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A15" s="14" t="s">
         <v>44</v>
       </c>
@@ -6284,7 +6283,7 @@
       <c r="T15" s="38"/>
       <c r="U15" s="38"/>
     </row>
-    <row r="16" spans="1:21" ht="17" customHeight="1">
+    <row r="16" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A16" s="14" t="s">
         <v>30</v>
       </c>
@@ -6477,7 +6476,7 @@
       <c r="T18" s="22"/>
       <c r="U18" s="22"/>
     </row>
-    <row r="19" spans="1:21" ht="17" customHeight="1">
+    <row r="19" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A19" s="14" t="s">
         <v>33</v>
       </c>
@@ -6540,7 +6539,7 @@
       <c r="T19" s="7"/>
       <c r="U19" s="7"/>
     </row>
-    <row r="20" spans="1:21" ht="17" customHeight="1">
+    <row r="20" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A20" s="14" t="s">
         <v>34</v>
       </c>
@@ -6606,7 +6605,7 @@
       <c r="T20" s="7"/>
       <c r="U20" s="7"/>
     </row>
-    <row r="21" spans="1:21" ht="17" customHeight="1">
+    <row r="21" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A21" s="14" t="s">
         <v>35</v>
       </c>
@@ -6669,7 +6668,7 @@
       <c r="T21" s="7"/>
       <c r="U21" s="7"/>
     </row>
-    <row r="22" spans="1:21" ht="17" customHeight="1">
+    <row r="22" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A22" s="14" t="s">
         <v>36</v>
       </c>
@@ -6730,7 +6729,7 @@
       <c r="T22" s="7"/>
       <c r="U22" s="7"/>
     </row>
-    <row r="23" spans="1:21" ht="17" customHeight="1">
+    <row r="23" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A23" s="14" t="s">
         <v>37</v>
       </c>
@@ -6794,7 +6793,7 @@
       <c r="T23" s="7"/>
       <c r="U23" s="7"/>
     </row>
-    <row r="24" spans="1:21" ht="17" customHeight="1">
+    <row r="24" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A24" s="14" t="s">
         <v>38</v>
       </c>
@@ -6857,7 +6856,7 @@
       <c r="T24" s="7"/>
       <c r="U24" s="7"/>
     </row>
-    <row r="25" spans="1:21" ht="17" customHeight="1">
+    <row r="25" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A25" s="14" t="s">
         <v>39</v>
       </c>
@@ -6917,7 +6916,7 @@
       <c r="T25" s="7"/>
       <c r="U25" s="7"/>
     </row>
-    <row r="26" spans="1:21" ht="17" customHeight="1">
+    <row r="26" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A26" s="14" t="s">
         <v>40</v>
       </c>
@@ -6979,7 +6978,7 @@
       <c r="T26" s="7"/>
       <c r="U26" s="7"/>
     </row>
-    <row r="27" spans="1:21" ht="17" customHeight="1">
+    <row r="27" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A27" s="14" t="s">
         <v>41</v>
       </c>
@@ -7066,15 +7065,15 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="12.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="12.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.46484375" style="27" customWidth="1"/>
-    <col min="2" max="2" width="10.86328125" style="27" customWidth="1"/>
-    <col min="3" max="21" width="9.19921875" style="27" customWidth="1"/>
-    <col min="22" max="256" width="8.86328125" style="27" customWidth="1"/>
+    <col min="1" max="1" width="43.42578125" style="27" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" style="27" customWidth="1"/>
+    <col min="3" max="21" width="9.140625" style="27" customWidth="1"/>
+    <col min="22" max="256" width="8.85546875" style="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="17" customHeight="1">
+    <row r="1" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -7105,7 +7104,7 @@
       <c r="T1" s="7"/>
       <c r="U1" s="7"/>
     </row>
-    <row r="2" spans="1:21" ht="17" customHeight="1">
+    <row r="2" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A2" s="8"/>
       <c r="B2" s="9"/>
       <c r="C2" s="9"/>
@@ -7247,7 +7246,7 @@
       <c r="T4" s="38"/>
       <c r="U4" s="38"/>
     </row>
-    <row r="5" spans="1:21" ht="17" customHeight="1">
+    <row r="5" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A5" s="18"/>
       <c r="B5" s="19"/>
       <c r="C5" s="20"/>
@@ -7270,7 +7269,7 @@
       <c r="T5" s="38"/>
       <c r="U5" s="38"/>
     </row>
-    <row r="6" spans="1:21" ht="17" customHeight="1">
+    <row r="6" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A6" s="14" t="s">
         <v>20</v>
       </c>
@@ -7336,7 +7335,7 @@
       <c r="T6" s="38"/>
       <c r="U6" s="38"/>
     </row>
-    <row r="7" spans="1:21" ht="17" customHeight="1">
+    <row r="7" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A7" s="14" t="s">
         <v>21</v>
       </c>
@@ -7402,7 +7401,7 @@
       <c r="T7" s="38"/>
       <c r="U7" s="38"/>
     </row>
-    <row r="8" spans="1:21" ht="17" customHeight="1">
+    <row r="8" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A8" s="14" t="s">
         <v>22</v>
       </c>
@@ -7468,7 +7467,7 @@
       <c r="T8" s="38"/>
       <c r="U8" s="38"/>
     </row>
-    <row r="9" spans="1:21" ht="17" customHeight="1">
+    <row r="9" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A9" s="14" t="s">
         <v>23</v>
       </c>
@@ -7534,7 +7533,7 @@
       <c r="T9" s="38"/>
       <c r="U9" s="38"/>
     </row>
-    <row r="10" spans="1:21" ht="17" customHeight="1">
+    <row r="10" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A10" s="14" t="s">
         <v>24</v>
       </c>
@@ -7600,7 +7599,7 @@
       <c r="T10" s="38"/>
       <c r="U10" s="38"/>
     </row>
-    <row r="11" spans="1:21" ht="17" customHeight="1">
+    <row r="11" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A11" s="14" t="s">
         <v>25</v>
       </c>
@@ -7666,7 +7665,7 @@
       <c r="T11" s="38"/>
       <c r="U11" s="38"/>
     </row>
-    <row r="12" spans="1:21" ht="17" customHeight="1">
+    <row r="12" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A12" s="14" t="s">
         <v>26</v>
       </c>
@@ -7732,7 +7731,7 @@
       <c r="T12" s="38"/>
       <c r="U12" s="38"/>
     </row>
-    <row r="13" spans="1:21" ht="17" customHeight="1">
+    <row r="13" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A13" s="14" t="s">
         <v>27</v>
       </c>
@@ -7798,7 +7797,7 @@
       <c r="T13" s="38"/>
       <c r="U13" s="38"/>
     </row>
-    <row r="14" spans="1:21" ht="17" customHeight="1">
+    <row r="14" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A14" s="14" t="s">
         <v>28</v>
       </c>
@@ -7861,7 +7860,7 @@
       <c r="T14" s="38"/>
       <c r="U14" s="38"/>
     </row>
-    <row r="15" spans="1:21" ht="17" customHeight="1">
+    <row r="15" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A15" s="14" t="s">
         <v>29</v>
       </c>
@@ -7925,7 +7924,7 @@
       <c r="T15" s="38"/>
       <c r="U15" s="38"/>
     </row>
-    <row r="16" spans="1:21" ht="17" customHeight="1">
+    <row r="16" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A16" s="14" t="s">
         <v>30</v>
       </c>
@@ -8118,7 +8117,7 @@
       <c r="T18" s="22"/>
       <c r="U18" s="22"/>
     </row>
-    <row r="19" spans="1:21" ht="17" customHeight="1">
+    <row r="19" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A19" s="14" t="s">
         <v>33</v>
       </c>
@@ -8181,7 +8180,7 @@
       <c r="T19" s="7"/>
       <c r="U19" s="7"/>
     </row>
-    <row r="20" spans="1:21" ht="17" customHeight="1">
+    <row r="20" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A20" s="14" t="s">
         <v>34</v>
       </c>
@@ -8247,7 +8246,7 @@
       <c r="T20" s="7"/>
       <c r="U20" s="7"/>
     </row>
-    <row r="21" spans="1:21" ht="17" customHeight="1">
+    <row r="21" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A21" s="14" t="s">
         <v>35</v>
       </c>
@@ -8313,7 +8312,7 @@
       <c r="T21" s="7"/>
       <c r="U21" s="7"/>
     </row>
-    <row r="22" spans="1:21" ht="17" customHeight="1">
+    <row r="22" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A22" s="14" t="s">
         <v>36</v>
       </c>
@@ -8377,7 +8376,7 @@
       <c r="T22" s="7"/>
       <c r="U22" s="7"/>
     </row>
-    <row r="23" spans="1:21" ht="17" customHeight="1">
+    <row r="23" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A23" s="14" t="s">
         <v>37</v>
       </c>
@@ -8443,7 +8442,7 @@
       <c r="T23" s="7"/>
       <c r="U23" s="7"/>
     </row>
-    <row r="24" spans="1:21" ht="17" customHeight="1">
+    <row r="24" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A24" s="14" t="s">
         <v>38</v>
       </c>
@@ -8509,7 +8508,7 @@
       <c r="T24" s="7"/>
       <c r="U24" s="7"/>
     </row>
-    <row r="25" spans="1:21" ht="17" customHeight="1">
+    <row r="25" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A25" s="14" t="s">
         <v>39</v>
       </c>
@@ -8575,7 +8574,7 @@
       <c r="T25" s="7"/>
       <c r="U25" s="7"/>
     </row>
-    <row r="26" spans="1:21" ht="17" customHeight="1">
+    <row r="26" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A26" s="14" t="s">
         <v>40</v>
       </c>
@@ -8641,7 +8640,7 @@
       <c r="T26" s="7"/>
       <c r="U26" s="7"/>
     </row>
-    <row r="27" spans="1:21" ht="17" customHeight="1">
+    <row r="27" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A27" s="14" t="s">
         <v>41</v>
       </c>
@@ -8728,15 +8727,15 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="12.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="12.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.46484375" style="28" customWidth="1"/>
-    <col min="2" max="2" width="10.86328125" style="28" customWidth="1"/>
-    <col min="3" max="21" width="9.19921875" style="28" customWidth="1"/>
-    <col min="22" max="256" width="8.86328125" style="28" customWidth="1"/>
+    <col min="1" max="1" width="43.42578125" style="28" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" style="28" customWidth="1"/>
+    <col min="3" max="21" width="9.140625" style="28" customWidth="1"/>
+    <col min="22" max="256" width="8.85546875" style="28" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="17" customHeight="1">
+    <row r="1" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -8767,7 +8766,7 @@
       <c r="T1" s="7"/>
       <c r="U1" s="7"/>
     </row>
-    <row r="2" spans="1:21" ht="17" customHeight="1">
+    <row r="2" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A2" s="8"/>
       <c r="B2" s="9"/>
       <c r="C2" s="9"/>
@@ -8901,7 +8900,7 @@
       <c r="T4" s="38"/>
       <c r="U4" s="38"/>
     </row>
-    <row r="5" spans="1:21" ht="17" customHeight="1">
+    <row r="5" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A5" s="18"/>
       <c r="B5" s="19"/>
       <c r="C5" s="20"/>
@@ -8924,7 +8923,7 @@
       <c r="T5" s="38"/>
       <c r="U5" s="38"/>
     </row>
-    <row r="6" spans="1:21" ht="17" customHeight="1">
+    <row r="6" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A6" s="14" t="s">
         <v>20</v>
       </c>
@@ -8990,7 +8989,7 @@
       <c r="T6" s="38"/>
       <c r="U6" s="38"/>
     </row>
-    <row r="7" spans="1:21" ht="17" customHeight="1">
+    <row r="7" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A7" s="14" t="s">
         <v>21</v>
       </c>
@@ -9056,7 +9055,7 @@
       <c r="T7" s="38"/>
       <c r="U7" s="38"/>
     </row>
-    <row r="8" spans="1:21" ht="17" customHeight="1">
+    <row r="8" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A8" s="14" t="s">
         <v>22</v>
       </c>
@@ -9122,7 +9121,7 @@
       <c r="T8" s="38"/>
       <c r="U8" s="38"/>
     </row>
-    <row r="9" spans="1:21" ht="17" customHeight="1">
+    <row r="9" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A9" s="14" t="s">
         <v>23</v>
       </c>
@@ -9188,7 +9187,7 @@
       <c r="T9" s="38"/>
       <c r="U9" s="38"/>
     </row>
-    <row r="10" spans="1:21" ht="17" customHeight="1">
+    <row r="10" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A10" s="14" t="s">
         <v>24</v>
       </c>
@@ -9254,7 +9253,7 @@
       <c r="T10" s="38"/>
       <c r="U10" s="38"/>
     </row>
-    <row r="11" spans="1:21" ht="17" customHeight="1">
+    <row r="11" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A11" s="14" t="s">
         <v>25</v>
       </c>
@@ -9320,7 +9319,7 @@
       <c r="T11" s="38"/>
       <c r="U11" s="38"/>
     </row>
-    <row r="12" spans="1:21" ht="17" customHeight="1">
+    <row r="12" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A12" s="14" t="s">
         <v>26</v>
       </c>
@@ -9386,7 +9385,7 @@
       <c r="T12" s="38"/>
       <c r="U12" s="38"/>
     </row>
-    <row r="13" spans="1:21" ht="17" customHeight="1">
+    <row r="13" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A13" s="14" t="s">
         <v>27</v>
       </c>
@@ -9452,7 +9451,7 @@
       <c r="T13" s="38"/>
       <c r="U13" s="38"/>
     </row>
-    <row r="14" spans="1:21" ht="17" customHeight="1">
+    <row r="14" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A14" s="14" t="s">
         <v>28</v>
       </c>
@@ -9518,7 +9517,7 @@
       <c r="T14" s="38"/>
       <c r="U14" s="38"/>
     </row>
-    <row r="15" spans="1:21" ht="17" customHeight="1">
+    <row r="15" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A15" s="14" t="s">
         <v>29</v>
       </c>
@@ -9584,7 +9583,7 @@
       <c r="T15" s="38"/>
       <c r="U15" s="38"/>
     </row>
-    <row r="16" spans="1:21" ht="17" customHeight="1">
+    <row r="16" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A16" s="14" t="s">
         <v>30</v>
       </c>
@@ -9778,7 +9777,7 @@
       <c r="T18" s="22"/>
       <c r="U18" s="22"/>
     </row>
-    <row r="19" spans="1:21" ht="17" customHeight="1">
+    <row r="19" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A19" s="14" t="s">
         <v>33</v>
       </c>
@@ -9841,7 +9840,7 @@
       <c r="T19" s="7"/>
       <c r="U19" s="7"/>
     </row>
-    <row r="20" spans="1:21" ht="17" customHeight="1">
+    <row r="20" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A20" s="14" t="s">
         <v>34</v>
       </c>
@@ -9907,7 +9906,7 @@
       <c r="T20" s="7"/>
       <c r="U20" s="7"/>
     </row>
-    <row r="21" spans="1:21" ht="17" customHeight="1">
+    <row r="21" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A21" s="14" t="s">
         <v>35</v>
       </c>
@@ -9973,7 +9972,7 @@
       <c r="T21" s="7"/>
       <c r="U21" s="7"/>
     </row>
-    <row r="22" spans="1:21" ht="17" customHeight="1">
+    <row r="22" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A22" s="14" t="s">
         <v>36</v>
       </c>
@@ -10039,7 +10038,7 @@
       <c r="T22" s="7"/>
       <c r="U22" s="7"/>
     </row>
-    <row r="23" spans="1:21" ht="17" customHeight="1">
+    <row r="23" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A23" s="14" t="s">
         <v>37</v>
       </c>
@@ -10105,7 +10104,7 @@
       <c r="T23" s="7"/>
       <c r="U23" s="7"/>
     </row>
-    <row r="24" spans="1:21" ht="17" customHeight="1">
+    <row r="24" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A24" s="14" t="s">
         <v>38</v>
       </c>
@@ -10171,7 +10170,7 @@
       <c r="T24" s="7"/>
       <c r="U24" s="7"/>
     </row>
-    <row r="25" spans="1:21" ht="17" customHeight="1">
+    <row r="25" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A25" s="14" t="s">
         <v>39</v>
       </c>
@@ -10237,7 +10236,7 @@
       <c r="T25" s="7"/>
       <c r="U25" s="7"/>
     </row>
-    <row r="26" spans="1:21" ht="17" customHeight="1">
+    <row r="26" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A26" s="14" t="s">
         <v>40</v>
       </c>
@@ -10302,7 +10301,7 @@
       <c r="T26" s="7"/>
       <c r="U26" s="7"/>
     </row>
-    <row r="27" spans="1:21" ht="17" customHeight="1">
+    <row r="27" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A27" s="14" t="s">
         <v>41</v>
       </c>
@@ -10389,15 +10388,15 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="12.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="12.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.46484375" style="29" customWidth="1"/>
-    <col min="2" max="2" width="10.86328125" style="29" customWidth="1"/>
-    <col min="3" max="21" width="9.19921875" style="29" customWidth="1"/>
-    <col min="22" max="256" width="8.86328125" style="29" customWidth="1"/>
+    <col min="1" max="1" width="43.42578125" style="29" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" style="29" customWidth="1"/>
+    <col min="3" max="21" width="9.140625" style="29" customWidth="1"/>
+    <col min="22" max="256" width="8.85546875" style="29" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="17" customHeight="1">
+    <row r="1" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -10428,7 +10427,7 @@
       <c r="T1" s="7"/>
       <c r="U1" s="7"/>
     </row>
-    <row r="2" spans="1:21" ht="17" customHeight="1">
+    <row r="2" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A2" s="8"/>
       <c r="B2" s="9"/>
       <c r="C2" s="9"/>
@@ -10563,7 +10562,7 @@
       <c r="T4" s="38"/>
       <c r="U4" s="38"/>
     </row>
-    <row r="5" spans="1:21" ht="17" customHeight="1">
+    <row r="5" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A5" s="18"/>
       <c r="B5" s="19"/>
       <c r="C5" s="20"/>
@@ -10586,7 +10585,7 @@
       <c r="T5" s="38"/>
       <c r="U5" s="38"/>
     </row>
-    <row r="6" spans="1:21" ht="17" customHeight="1">
+    <row r="6" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A6" s="14" t="s">
         <v>20</v>
       </c>
@@ -10650,7 +10649,7 @@
       <c r="T6" s="38"/>
       <c r="U6" s="38"/>
     </row>
-    <row r="7" spans="1:21" ht="17" customHeight="1">
+    <row r="7" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A7" s="14" t="s">
         <v>21</v>
       </c>
@@ -10716,7 +10715,7 @@
       <c r="T7" s="38"/>
       <c r="U7" s="38"/>
     </row>
-    <row r="8" spans="1:21" ht="17" customHeight="1">
+    <row r="8" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A8" s="14" t="s">
         <v>22</v>
       </c>
@@ -10779,7 +10778,7 @@
       <c r="T8" s="38"/>
       <c r="U8" s="38"/>
     </row>
-    <row r="9" spans="1:21" ht="17" customHeight="1">
+    <row r="9" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A9" s="14" t="s">
         <v>23</v>
       </c>
@@ -10845,7 +10844,7 @@
       <c r="T9" s="38"/>
       <c r="U9" s="38"/>
     </row>
-    <row r="10" spans="1:21" ht="17" customHeight="1">
+    <row r="10" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A10" s="14" t="s">
         <v>24</v>
       </c>
@@ -10911,7 +10910,7 @@
       <c r="T10" s="38"/>
       <c r="U10" s="38"/>
     </row>
-    <row r="11" spans="1:21" ht="17" customHeight="1">
+    <row r="11" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A11" s="14" t="s">
         <v>25</v>
       </c>
@@ -10977,7 +10976,7 @@
       <c r="T11" s="38"/>
       <c r="U11" s="38"/>
     </row>
-    <row r="12" spans="1:21" ht="17" customHeight="1">
+    <row r="12" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A12" s="14" t="s">
         <v>26</v>
       </c>
@@ -11043,7 +11042,7 @@
       <c r="T12" s="38"/>
       <c r="U12" s="38"/>
     </row>
-    <row r="13" spans="1:21" ht="17" customHeight="1">
+    <row r="13" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A13" s="14" t="s">
         <v>27</v>
       </c>
@@ -11109,7 +11108,7 @@
       <c r="T13" s="38"/>
       <c r="U13" s="38"/>
     </row>
-    <row r="14" spans="1:21" ht="17" customHeight="1">
+    <row r="14" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A14" s="14" t="s">
         <v>28</v>
       </c>
@@ -11175,7 +11174,7 @@
       <c r="T14" s="38"/>
       <c r="U14" s="38"/>
     </row>
-    <row r="15" spans="1:21" ht="17" customHeight="1">
+    <row r="15" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A15" s="14" t="s">
         <v>29</v>
       </c>
@@ -11241,7 +11240,7 @@
       <c r="T15" s="38"/>
       <c r="U15" s="38"/>
     </row>
-    <row r="16" spans="1:21" ht="17" customHeight="1">
+    <row r="16" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A16" s="14" t="s">
         <v>30</v>
       </c>
@@ -11436,7 +11435,7 @@
       <c r="T18" s="22"/>
       <c r="U18" s="22"/>
     </row>
-    <row r="19" spans="1:21" ht="17" customHeight="1">
+    <row r="19" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A19" s="14" t="s">
         <v>33</v>
       </c>
@@ -11502,7 +11501,7 @@
       <c r="T19" s="7"/>
       <c r="U19" s="7"/>
     </row>
-    <row r="20" spans="1:21" ht="17" customHeight="1">
+    <row r="20" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A20" s="14" t="s">
         <v>34</v>
       </c>
@@ -11565,7 +11564,7 @@
       <c r="T20" s="7"/>
       <c r="U20" s="7"/>
     </row>
-    <row r="21" spans="1:21" ht="17" customHeight="1">
+    <row r="21" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A21" s="14" t="s">
         <v>35</v>
       </c>
@@ -11627,7 +11626,7 @@
       <c r="T21" s="7"/>
       <c r="U21" s="7"/>
     </row>
-    <row r="22" spans="1:21" ht="17" customHeight="1">
+    <row r="22" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A22" s="14" t="s">
         <v>36</v>
       </c>
@@ -11692,7 +11691,7 @@
       <c r="T22" s="7"/>
       <c r="U22" s="7"/>
     </row>
-    <row r="23" spans="1:21" ht="17" customHeight="1">
+    <row r="23" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A23" s="14" t="s">
         <v>37</v>
       </c>
@@ -11758,7 +11757,7 @@
       <c r="T23" s="7"/>
       <c r="U23" s="7"/>
     </row>
-    <row r="24" spans="1:21" ht="17" customHeight="1">
+    <row r="24" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A24" s="14" t="s">
         <v>38</v>
       </c>
@@ -11824,7 +11823,7 @@
       <c r="T24" s="7"/>
       <c r="U24" s="7"/>
     </row>
-    <row r="25" spans="1:21" ht="17" customHeight="1">
+    <row r="25" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A25" s="14" t="s">
         <v>39</v>
       </c>
@@ -11888,7 +11887,7 @@
       <c r="T25" s="7"/>
       <c r="U25" s="7"/>
     </row>
-    <row r="26" spans="1:21" ht="17" customHeight="1">
+    <row r="26" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A26" s="14" t="s">
         <v>40</v>
       </c>
@@ -11951,7 +11950,7 @@
       <c r="T26" s="7"/>
       <c r="U26" s="7"/>
     </row>
-    <row r="27" spans="1:21" ht="17" customHeight="1">
+    <row r="27" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A27" s="14" t="s">
         <v>41</v>
       </c>
@@ -12036,17 +12035,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:IV28"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:C1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="12.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="12.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.46484375" style="30" customWidth="1"/>
-    <col min="2" max="2" width="10.86328125" style="30" customWidth="1"/>
-    <col min="3" max="21" width="9.19921875" style="30" customWidth="1"/>
-    <col min="22" max="256" width="8.86328125" style="30" customWidth="1"/>
+    <col min="1" max="1" width="43.42578125" style="30" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" style="30" customWidth="1"/>
+    <col min="3" max="21" width="9.140625" style="30" customWidth="1"/>
+    <col min="22" max="256" width="8.85546875" style="30" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="17" customHeight="1">
+    <row r="1" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -12077,7 +12078,7 @@
       <c r="T1" s="7"/>
       <c r="U1" s="7"/>
     </row>
-    <row r="2" spans="1:21" ht="17" customHeight="1">
+    <row r="2" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A2" s="8"/>
       <c r="B2" s="9"/>
       <c r="C2" s="9"/>
@@ -12218,7 +12219,7 @@
       <c r="T4" s="38"/>
       <c r="U4" s="38"/>
     </row>
-    <row r="5" spans="1:21" ht="17" customHeight="1">
+    <row r="5" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A5" s="18"/>
       <c r="B5" s="19"/>
       <c r="C5" s="20"/>
@@ -12241,7 +12242,7 @@
       <c r="T5" s="38"/>
       <c r="U5" s="38"/>
     </row>
-    <row r="6" spans="1:21" ht="17" customHeight="1">
+    <row r="6" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A6" s="14" t="s">
         <v>20</v>
       </c>
@@ -12306,7 +12307,7 @@
       <c r="T6" s="38"/>
       <c r="U6" s="38"/>
     </row>
-    <row r="7" spans="1:21" ht="17" customHeight="1">
+    <row r="7" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A7" s="14" t="s">
         <v>21</v>
       </c>
@@ -12372,7 +12373,7 @@
       <c r="T7" s="38"/>
       <c r="U7" s="38"/>
     </row>
-    <row r="8" spans="1:21" ht="17" customHeight="1">
+    <row r="8" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A8" s="14" t="s">
         <v>22</v>
       </c>
@@ -12438,7 +12439,7 @@
       <c r="T8" s="38"/>
       <c r="U8" s="38"/>
     </row>
-    <row r="9" spans="1:21" ht="17" customHeight="1">
+    <row r="9" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A9" s="14" t="s">
         <v>23</v>
       </c>
@@ -12504,7 +12505,7 @@
       <c r="T9" s="38"/>
       <c r="U9" s="38"/>
     </row>
-    <row r="10" spans="1:21" ht="17" customHeight="1">
+    <row r="10" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A10" s="14" t="s">
         <v>24</v>
       </c>
@@ -12570,7 +12571,7 @@
       <c r="T10" s="38"/>
       <c r="U10" s="38"/>
     </row>
-    <row r="11" spans="1:21" ht="17" customHeight="1">
+    <row r="11" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A11" s="14" t="s">
         <v>25</v>
       </c>
@@ -12636,7 +12637,7 @@
       <c r="T11" s="38"/>
       <c r="U11" s="38"/>
     </row>
-    <row r="12" spans="1:21" ht="17" customHeight="1">
+    <row r="12" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A12" s="14" t="s">
         <v>26</v>
       </c>
@@ -12701,7 +12702,7 @@
       <c r="T12" s="38"/>
       <c r="U12" s="38"/>
     </row>
-    <row r="13" spans="1:21" ht="17" customHeight="1">
+    <row r="13" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A13" s="14" t="s">
         <v>27</v>
       </c>
@@ -12767,7 +12768,7 @@
       <c r="T13" s="38"/>
       <c r="U13" s="38"/>
     </row>
-    <row r="14" spans="1:21" ht="17" customHeight="1">
+    <row r="14" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A14" s="14" t="s">
         <v>28</v>
       </c>
@@ -12833,7 +12834,7 @@
       <c r="T14" s="38"/>
       <c r="U14" s="38"/>
     </row>
-    <row r="15" spans="1:21" ht="17" customHeight="1">
+    <row r="15" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A15" s="14" t="s">
         <v>29</v>
       </c>
@@ -12899,7 +12900,7 @@
       <c r="T15" s="38"/>
       <c r="U15" s="38"/>
     </row>
-    <row r="16" spans="1:21" ht="17" customHeight="1">
+    <row r="16" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A16" s="14" t="s">
         <v>30</v>
       </c>
@@ -13095,7 +13096,7 @@
       <c r="T18" s="22"/>
       <c r="U18" s="22"/>
     </row>
-    <row r="19" spans="1:21" ht="17" customHeight="1">
+    <row r="19" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A19" s="14" t="s">
         <v>33</v>
       </c>
@@ -13158,7 +13159,7 @@
       <c r="T19" s="7"/>
       <c r="U19" s="7"/>
     </row>
-    <row r="20" spans="1:21" ht="17" customHeight="1">
+    <row r="20" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A20" s="14" t="s">
         <v>34</v>
       </c>
@@ -13224,7 +13225,7 @@
       <c r="T20" s="7"/>
       <c r="U20" s="7"/>
     </row>
-    <row r="21" spans="1:21" ht="17" customHeight="1">
+    <row r="21" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A21" s="14" t="s">
         <v>35</v>
       </c>
@@ -13290,7 +13291,7 @@
       <c r="T21" s="7"/>
       <c r="U21" s="7"/>
     </row>
-    <row r="22" spans="1:21" ht="17" customHeight="1">
+    <row r="22" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A22" s="14" t="s">
         <v>36</v>
       </c>
@@ -13356,7 +13357,7 @@
       <c r="T22" s="7"/>
       <c r="U22" s="7"/>
     </row>
-    <row r="23" spans="1:21" ht="17" customHeight="1">
+    <row r="23" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A23" s="14" t="s">
         <v>37</v>
       </c>
@@ -13422,7 +13423,7 @@
       <c r="T23" s="7"/>
       <c r="U23" s="7"/>
     </row>
-    <row r="24" spans="1:21" ht="17" customHeight="1">
+    <row r="24" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A24" s="14" t="s">
         <v>38</v>
       </c>
@@ -13488,7 +13489,7 @@
       <c r="T24" s="7"/>
       <c r="U24" s="7"/>
     </row>
-    <row r="25" spans="1:21" ht="17" customHeight="1">
+    <row r="25" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A25" s="14" t="s">
         <v>39</v>
       </c>
@@ -13554,7 +13555,7 @@
       <c r="T25" s="7"/>
       <c r="U25" s="7"/>
     </row>
-    <row r="26" spans="1:21" ht="17" customHeight="1">
+    <row r="26" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A26" s="14" t="s">
         <v>40</v>
       </c>
@@ -13620,7 +13621,7 @@
       <c r="T26" s="7"/>
       <c r="U26" s="7"/>
     </row>
-    <row r="27" spans="1:21" ht="17" customHeight="1">
+    <row r="27" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A27" s="14" t="s">
         <v>41</v>
       </c>
@@ -13686,7 +13687,7 @@
       <c r="T27" s="7"/>
       <c r="U27" s="7"/>
     </row>
-    <row r="28" spans="1:21" ht="17" customHeight="1">
+    <row r="28" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A28" s="14" t="s">
         <v>41</v>
       </c>
@@ -13773,15 +13774,15 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="12.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="12.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.46484375" style="31" customWidth="1"/>
-    <col min="2" max="2" width="10.86328125" style="31" customWidth="1"/>
-    <col min="3" max="21" width="9.19921875" style="31" customWidth="1"/>
-    <col min="22" max="256" width="8.86328125" style="31" customWidth="1"/>
+    <col min="1" max="1" width="43.42578125" style="31" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" style="31" customWidth="1"/>
+    <col min="3" max="21" width="9.140625" style="31" customWidth="1"/>
+    <col min="22" max="256" width="8.85546875" style="31" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="17" customHeight="1">
+    <row r="1" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -13812,7 +13813,7 @@
       <c r="T1" s="7"/>
       <c r="U1" s="7"/>
     </row>
-    <row r="2" spans="1:21" ht="17" customHeight="1">
+    <row r="2" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A2" s="8"/>
       <c r="B2" s="9"/>
       <c r="C2" s="9"/>
@@ -13943,7 +13944,7 @@
       <c r="T4" s="38"/>
       <c r="U4" s="38"/>
     </row>
-    <row r="5" spans="1:21" ht="17" customHeight="1">
+    <row r="5" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A5" s="18"/>
       <c r="B5" s="19"/>
       <c r="C5" s="20"/>
@@ -13966,7 +13967,7 @@
       <c r="T5" s="38"/>
       <c r="U5" s="38"/>
     </row>
-    <row r="6" spans="1:21" ht="17" customHeight="1">
+    <row r="6" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A6" s="14" t="s">
         <v>20</v>
       </c>
@@ -14019,7 +14020,7 @@
       <c r="T6" s="38"/>
       <c r="U6" s="38"/>
     </row>
-    <row r="7" spans="1:21" ht="17" customHeight="1">
+    <row r="7" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A7" s="14" t="s">
         <v>21</v>
       </c>
@@ -14082,7 +14083,7 @@
       <c r="T7" s="38"/>
       <c r="U7" s="38"/>
     </row>
-    <row r="8" spans="1:21" ht="17" customHeight="1">
+    <row r="8" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A8" s="14" t="s">
         <v>22</v>
       </c>
@@ -14148,7 +14149,7 @@
       <c r="T8" s="38"/>
       <c r="U8" s="38"/>
     </row>
-    <row r="9" spans="1:21" ht="17" customHeight="1">
+    <row r="9" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A9" s="14" t="s">
         <v>23</v>
       </c>
@@ -14212,7 +14213,7 @@
       <c r="T9" s="38"/>
       <c r="U9" s="38"/>
     </row>
-    <row r="10" spans="1:21" ht="17" customHeight="1">
+    <row r="10" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A10" s="14" t="s">
         <v>24</v>
       </c>
@@ -14271,7 +14272,7 @@
       <c r="T10" s="38"/>
       <c r="U10" s="38"/>
     </row>
-    <row r="11" spans="1:21" ht="17" customHeight="1">
+    <row r="11" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A11" s="14" t="s">
         <v>25</v>
       </c>
@@ -14333,7 +14334,7 @@
       <c r="T11" s="38"/>
       <c r="U11" s="38"/>
     </row>
-    <row r="12" spans="1:21" ht="17" customHeight="1">
+    <row r="12" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A12" s="14" t="s">
         <v>26</v>
       </c>
@@ -14399,7 +14400,7 @@
       <c r="T12" s="38"/>
       <c r="U12" s="38"/>
     </row>
-    <row r="13" spans="1:21" ht="17" customHeight="1">
+    <row r="13" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A13" s="14" t="s">
         <v>27</v>
       </c>
@@ -14459,7 +14460,7 @@
       <c r="T13" s="38"/>
       <c r="U13" s="38"/>
     </row>
-    <row r="14" spans="1:21" ht="17" customHeight="1">
+    <row r="14" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A14" s="14" t="s">
         <v>28</v>
       </c>
@@ -14525,7 +14526,7 @@
       <c r="T14" s="38"/>
       <c r="U14" s="38"/>
     </row>
-    <row r="15" spans="1:21" ht="17" customHeight="1">
+    <row r="15" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A15" s="14" t="s">
         <v>29</v>
       </c>
@@ -14589,7 +14590,7 @@
       <c r="T15" s="38"/>
       <c r="U15" s="38"/>
     </row>
-    <row r="16" spans="1:21" ht="17" customHeight="1">
+    <row r="16" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A16" s="14" t="s">
         <v>30</v>
       </c>
@@ -14783,7 +14784,7 @@
       <c r="T18" s="22"/>
       <c r="U18" s="22"/>
     </row>
-    <row r="19" spans="1:21" ht="17" customHeight="1">
+    <row r="19" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A19" s="14" t="s">
         <v>33</v>
       </c>
@@ -14849,7 +14850,7 @@
       <c r="T19" s="7"/>
       <c r="U19" s="7"/>
     </row>
-    <row r="20" spans="1:21" ht="17" customHeight="1">
+    <row r="20" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A20" s="14" t="s">
         <v>34</v>
       </c>
@@ -14915,7 +14916,7 @@
       <c r="T20" s="7"/>
       <c r="U20" s="7"/>
     </row>
-    <row r="21" spans="1:21" ht="17" customHeight="1">
+    <row r="21" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A21" s="14" t="s">
         <v>35</v>
       </c>
@@ -14980,7 +14981,7 @@
       <c r="T21" s="7"/>
       <c r="U21" s="7"/>
     </row>
-    <row r="22" spans="1:21" ht="17" customHeight="1">
+    <row r="22" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A22" s="14" t="s">
         <v>36</v>
       </c>
@@ -15046,7 +15047,7 @@
       <c r="T22" s="7"/>
       <c r="U22" s="7"/>
     </row>
-    <row r="23" spans="1:21" ht="17" customHeight="1">
+    <row r="23" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A23" s="14" t="s">
         <v>37</v>
       </c>
@@ -15112,7 +15113,7 @@
       <c r="T23" s="7"/>
       <c r="U23" s="7"/>
     </row>
-    <row r="24" spans="1:21" ht="17" customHeight="1">
+    <row r="24" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A24" s="14" t="s">
         <v>38</v>
       </c>
@@ -15178,7 +15179,7 @@
       <c r="T24" s="7"/>
       <c r="U24" s="7"/>
     </row>
-    <row r="25" spans="1:21" ht="17" customHeight="1">
+    <row r="25" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A25" s="14" t="s">
         <v>39</v>
       </c>
@@ -15242,7 +15243,7 @@
       <c r="T25" s="7"/>
       <c r="U25" s="7"/>
     </row>
-    <row r="26" spans="1:21" ht="17" customHeight="1">
+    <row r="26" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A26" s="14" t="s">
         <v>40</v>
       </c>
@@ -15306,7 +15307,7 @@
       <c r="T26" s="7"/>
       <c r="U26" s="7"/>
     </row>
-    <row r="27" spans="1:21" ht="17" customHeight="1">
+    <row r="27" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A27" s="14" t="s">
         <v>41</v>
       </c>
@@ -15393,15 +15394,15 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="12.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="12.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.46484375" style="32" customWidth="1"/>
-    <col min="2" max="2" width="10.86328125" style="32" customWidth="1"/>
-    <col min="3" max="21" width="9.19921875" style="32" customWidth="1"/>
-    <col min="22" max="256" width="8.86328125" style="32" customWidth="1"/>
+    <col min="1" max="1" width="43.42578125" style="32" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" style="32" customWidth="1"/>
+    <col min="3" max="21" width="9.140625" style="32" customWidth="1"/>
+    <col min="22" max="256" width="8.85546875" style="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="17" customHeight="1">
+    <row r="1" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -15432,7 +15433,7 @@
       <c r="T1" s="7"/>
       <c r="U1" s="7"/>
     </row>
-    <row r="2" spans="1:21" ht="17" customHeight="1">
+    <row r="2" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A2" s="8"/>
       <c r="B2" s="9"/>
       <c r="C2" s="9"/>
@@ -15567,7 +15568,7 @@
       <c r="T4" s="38"/>
       <c r="U4" s="38"/>
     </row>
-    <row r="5" spans="1:21" ht="17" customHeight="1">
+    <row r="5" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A5" s="18"/>
       <c r="B5" s="19"/>
       <c r="C5" s="20"/>
@@ -15590,7 +15591,7 @@
       <c r="T5" s="38"/>
       <c r="U5" s="38"/>
     </row>
-    <row r="6" spans="1:21" ht="17" customHeight="1">
+    <row r="6" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A6" s="14" t="s">
         <v>20</v>
       </c>
@@ -15648,7 +15649,7 @@
       <c r="T6" s="38"/>
       <c r="U6" s="38"/>
     </row>
-    <row r="7" spans="1:21" ht="17" customHeight="1">
+    <row r="7" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A7" s="14" t="s">
         <v>21</v>
       </c>
@@ -15714,7 +15715,7 @@
       <c r="T7" s="38"/>
       <c r="U7" s="38"/>
     </row>
-    <row r="8" spans="1:21" ht="17" customHeight="1">
+    <row r="8" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A8" s="14" t="s">
         <v>22</v>
       </c>
@@ -15780,7 +15781,7 @@
       <c r="T8" s="38"/>
       <c r="U8" s="38"/>
     </row>
-    <row r="9" spans="1:21" ht="17" customHeight="1">
+    <row r="9" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A9" s="14" t="s">
         <v>23</v>
       </c>
@@ -15841,7 +15842,7 @@
       <c r="T9" s="38"/>
       <c r="U9" s="38"/>
     </row>
-    <row r="10" spans="1:21" ht="17" customHeight="1">
+    <row r="10" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A10" s="14" t="s">
         <v>24</v>
       </c>
@@ -15901,7 +15902,7 @@
       <c r="T10" s="38"/>
       <c r="U10" s="38"/>
     </row>
-    <row r="11" spans="1:21" ht="17" customHeight="1">
+    <row r="11" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A11" s="14" t="s">
         <v>25</v>
       </c>
@@ -15967,7 +15968,7 @@
       <c r="T11" s="38"/>
       <c r="U11" s="38"/>
     </row>
-    <row r="12" spans="1:21" ht="17" customHeight="1">
+    <row r="12" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A12" s="14" t="s">
         <v>26</v>
       </c>
@@ -16027,7 +16028,7 @@
       <c r="T12" s="38"/>
       <c r="U12" s="38"/>
     </row>
-    <row r="13" spans="1:21" ht="17" customHeight="1">
+    <row r="13" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A13" s="14" t="s">
         <v>27</v>
       </c>
@@ -16089,7 +16090,7 @@
       <c r="T13" s="38"/>
       <c r="U13" s="38"/>
     </row>
-    <row r="14" spans="1:21" ht="17" customHeight="1">
+    <row r="14" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A14" s="14" t="s">
         <v>28</v>
       </c>
@@ -16151,7 +16152,7 @@
       <c r="T14" s="38"/>
       <c r="U14" s="38"/>
     </row>
-    <row r="15" spans="1:21" ht="17" customHeight="1">
+    <row r="15" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A15" s="14" t="s">
         <v>29</v>
       </c>
@@ -16217,7 +16218,7 @@
       <c r="T15" s="38"/>
       <c r="U15" s="38"/>
     </row>
-    <row r="16" spans="1:21" ht="17" customHeight="1">
+    <row r="16" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A16" s="14" t="s">
         <v>30</v>
       </c>
@@ -16395,7 +16396,7 @@
       <c r="T18" s="22"/>
       <c r="U18" s="22"/>
     </row>
-    <row r="19" spans="1:21" ht="17" customHeight="1">
+    <row r="19" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A19" s="14" t="s">
         <v>33</v>
       </c>
@@ -16458,7 +16459,7 @@
       <c r="T19" s="7"/>
       <c r="U19" s="7"/>
     </row>
-    <row r="20" spans="1:21" ht="17" customHeight="1">
+    <row r="20" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A20" s="14" t="s">
         <v>34</v>
       </c>
@@ -16524,7 +16525,7 @@
       <c r="T20" s="7"/>
       <c r="U20" s="7"/>
     </row>
-    <row r="21" spans="1:21" ht="17" customHeight="1">
+    <row r="21" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A21" s="14" t="s">
         <v>35</v>
       </c>
@@ -16590,7 +16591,7 @@
       <c r="T21" s="7"/>
       <c r="U21" s="7"/>
     </row>
-    <row r="22" spans="1:21" ht="17" customHeight="1">
+    <row r="22" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A22" s="14" t="s">
         <v>36</v>
       </c>
@@ -16653,7 +16654,7 @@
       <c r="T22" s="7"/>
       <c r="U22" s="7"/>
     </row>
-    <row r="23" spans="1:21" ht="17" customHeight="1">
+    <row r="23" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A23" s="14" t="s">
         <v>37</v>
       </c>
@@ -16716,7 +16717,7 @@
       <c r="T23" s="7"/>
       <c r="U23" s="7"/>
     </row>
-    <row r="24" spans="1:21" ht="17" customHeight="1">
+    <row r="24" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A24" s="14" t="s">
         <v>38</v>
       </c>
@@ -16782,7 +16783,7 @@
       <c r="T24" s="7"/>
       <c r="U24" s="7"/>
     </row>
-    <row r="25" spans="1:21" ht="17" customHeight="1">
+    <row r="25" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A25" s="14" t="s">
         <v>39</v>
       </c>
@@ -16848,7 +16849,7 @@
       <c r="T25" s="7"/>
       <c r="U25" s="7"/>
     </row>
-    <row r="26" spans="1:21" ht="17" customHeight="1">
+    <row r="26" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A26" s="14" t="s">
         <v>40</v>
       </c>
@@ -16914,7 +16915,7 @@
       <c r="T26" s="7"/>
       <c r="U26" s="7"/>
     </row>
-    <row r="27" spans="1:21" ht="17" customHeight="1">
+    <row r="27" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A27" s="14" t="s">
         <v>41</v>
       </c>
@@ -17001,15 +17002,15 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="12.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="12.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.46484375" style="33" customWidth="1"/>
-    <col min="2" max="2" width="10.86328125" style="33" customWidth="1"/>
-    <col min="3" max="21" width="9.19921875" style="33" customWidth="1"/>
-    <col min="22" max="256" width="8.86328125" style="33" customWidth="1"/>
+    <col min="1" max="1" width="43.42578125" style="33" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" style="33" customWidth="1"/>
+    <col min="3" max="21" width="9.140625" style="33" customWidth="1"/>
+    <col min="22" max="256" width="8.85546875" style="33" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="17" customHeight="1">
+    <row r="1" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -17040,7 +17041,7 @@
       <c r="T1" s="7"/>
       <c r="U1" s="7"/>
     </row>
-    <row r="2" spans="1:21" ht="17" customHeight="1">
+    <row r="2" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A2" s="8"/>
       <c r="B2" s="9"/>
       <c r="C2" s="9"/>
@@ -17181,7 +17182,7 @@
       <c r="T4" s="38"/>
       <c r="U4" s="38"/>
     </row>
-    <row r="5" spans="1:21" ht="17" customHeight="1">
+    <row r="5" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A5" s="18"/>
       <c r="B5" s="19"/>
       <c r="C5" s="20"/>
@@ -17204,7 +17205,7 @@
       <c r="T5" s="38"/>
       <c r="U5" s="38"/>
     </row>
-    <row r="6" spans="1:21" ht="17" customHeight="1">
+    <row r="6" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A6" s="14" t="s">
         <v>20</v>
       </c>
@@ -17270,7 +17271,7 @@
       <c r="T6" s="38"/>
       <c r="U6" s="38"/>
     </row>
-    <row r="7" spans="1:21" ht="17" customHeight="1">
+    <row r="7" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A7" s="14" t="s">
         <v>21</v>
       </c>
@@ -17336,7 +17337,7 @@
       <c r="T7" s="38"/>
       <c r="U7" s="38"/>
     </row>
-    <row r="8" spans="1:21" ht="17" customHeight="1">
+    <row r="8" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A8" s="14" t="s">
         <v>22</v>
       </c>
@@ -17401,7 +17402,7 @@
       <c r="T8" s="38"/>
       <c r="U8" s="38"/>
     </row>
-    <row r="9" spans="1:21" ht="17" customHeight="1">
+    <row r="9" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A9" s="14" t="s">
         <v>23</v>
       </c>
@@ -17467,7 +17468,7 @@
       <c r="T9" s="38"/>
       <c r="U9" s="38"/>
     </row>
-    <row r="10" spans="1:21" ht="17" customHeight="1">
+    <row r="10" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A10" s="14" t="s">
         <v>24</v>
       </c>
@@ -17533,7 +17534,7 @@
       <c r="T10" s="38"/>
       <c r="U10" s="38"/>
     </row>
-    <row r="11" spans="1:21" ht="17" customHeight="1">
+    <row r="11" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A11" s="14" t="s">
         <v>25</v>
       </c>
@@ -17599,7 +17600,7 @@
       <c r="T11" s="38"/>
       <c r="U11" s="38"/>
     </row>
-    <row r="12" spans="1:21" ht="17" customHeight="1">
+    <row r="12" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A12" s="14" t="s">
         <v>26</v>
       </c>
@@ -17665,7 +17666,7 @@
       <c r="T12" s="38"/>
       <c r="U12" s="38"/>
     </row>
-    <row r="13" spans="1:21" ht="17" customHeight="1">
+    <row r="13" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A13" s="14" t="s">
         <v>27</v>
       </c>
@@ -17731,7 +17732,7 @@
       <c r="T13" s="38"/>
       <c r="U13" s="38"/>
     </row>
-    <row r="14" spans="1:21" ht="17" customHeight="1">
+    <row r="14" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A14" s="14" t="s">
         <v>28</v>
       </c>
@@ -17797,7 +17798,7 @@
       <c r="T14" s="38"/>
       <c r="U14" s="38"/>
     </row>
-    <row r="15" spans="1:21" ht="17" customHeight="1">
+    <row r="15" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A15" s="14" t="s">
         <v>29</v>
       </c>
@@ -17863,7 +17864,7 @@
       <c r="T15" s="38"/>
       <c r="U15" s="38"/>
     </row>
-    <row r="16" spans="1:21" ht="17" customHeight="1">
+    <row r="16" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A16" s="14" t="s">
         <v>30</v>
       </c>
@@ -18061,7 +18062,7 @@
       <c r="T18" s="22"/>
       <c r="U18" s="22"/>
     </row>
-    <row r="19" spans="1:21" ht="17" customHeight="1">
+    <row r="19" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A19" s="14" t="s">
         <v>33</v>
       </c>
@@ -18127,7 +18128,7 @@
       <c r="T19" s="7"/>
       <c r="U19" s="7"/>
     </row>
-    <row r="20" spans="1:21" ht="17" customHeight="1">
+    <row r="20" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A20" s="14" t="s">
         <v>34</v>
       </c>
@@ -18193,7 +18194,7 @@
       <c r="T20" s="7"/>
       <c r="U20" s="7"/>
     </row>
-    <row r="21" spans="1:21" ht="17" customHeight="1">
+    <row r="21" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A21" s="14" t="s">
         <v>35</v>
       </c>
@@ -18259,7 +18260,7 @@
       <c r="T21" s="7"/>
       <c r="U21" s="7"/>
     </row>
-    <row r="22" spans="1:21" ht="17" customHeight="1">
+    <row r="22" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A22" s="14" t="s">
         <v>36</v>
       </c>
@@ -18325,7 +18326,7 @@
       <c r="T22" s="7"/>
       <c r="U22" s="7"/>
     </row>
-    <row r="23" spans="1:21" ht="17" customHeight="1">
+    <row r="23" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A23" s="14" t="s">
         <v>37</v>
       </c>
@@ -18391,7 +18392,7 @@
       <c r="T23" s="7"/>
       <c r="U23" s="7"/>
     </row>
-    <row r="24" spans="1:21" ht="17" customHeight="1">
+    <row r="24" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A24" s="14" t="s">
         <v>38</v>
       </c>
@@ -18457,7 +18458,7 @@
       <c r="T24" s="7"/>
       <c r="U24" s="7"/>
     </row>
-    <row r="25" spans="1:21" ht="17" customHeight="1">
+    <row r="25" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A25" s="14" t="s">
         <v>39</v>
       </c>
@@ -18523,7 +18524,7 @@
       <c r="T25" s="7"/>
       <c r="U25" s="7"/>
     </row>
-    <row r="26" spans="1:21" ht="17" customHeight="1">
+    <row r="26" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A26" s="14" t="s">
         <v>40</v>
       </c>
@@ -18589,7 +18590,7 @@
       <c r="T26" s="7"/>
       <c r="U26" s="7"/>
     </row>
-    <row r="27" spans="1:21" ht="17" customHeight="1">
+    <row r="27" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A27" s="14" t="s">
         <v>41</v>
       </c>

</xml_diff>